<commit_message>
Fixed plots and initial data
Results for 2020 in EG adjusted to real data
Fixed some colours in the plots
Added detailed plot of water consumption for hydro
</commit_message>
<xml_diff>
--- a/debugging/results/results_check.xlsx
+++ b/debugging/results/results_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessandro Pieruzzi\Documents\Thesis\TEMBA_FPV\debugging\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F82089-5E0A-494A-986E-C4D0D2154621}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58EE3336-7CE0-4CCA-A7AE-10B9864083FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EG" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>Oil</t>
   </si>
@@ -90,13 +90,37 @@
   </si>
   <si>
     <t xml:space="preserve">total </t>
+  </si>
+  <si>
+    <t>CAPACITY</t>
+  </si>
+  <si>
+    <t>Modeled (GW)</t>
+  </si>
+  <si>
+    <t>Actual (GW)</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source: </t>
+  </si>
+  <si>
+    <t>http://www.moee.gov.eg/english_new/EEHC_Rep/REP2021-2022en.pdf</t>
+  </si>
+  <si>
+    <t>Difference</t>
+  </si>
+  <si>
+    <t>Fossil</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +138,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -168,10 +200,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -186,14 +219,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,16 +523,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
@@ -536,7 +565,7 @@
         <v>7.57</v>
       </c>
       <c r="C2" s="3">
-        <f>B2*$C$11</f>
+        <f t="shared" ref="C2:C7" si="0">B2*$C$11</f>
         <v>2102.7188999999998</v>
       </c>
       <c r="D2" s="3">
@@ -547,7 +576,7 @@
         <v>-5044.2811000000002</v>
       </c>
       <c r="F2">
-        <f>E2/$C$11</f>
+        <f t="shared" ref="F2:F8" si="1">E2/$C$11</f>
         <v>-18.159920437772261</v>
       </c>
     </row>
@@ -559,18 +588,18 @@
         <v>509.01</v>
       </c>
       <c r="C3" s="3">
-        <f>B3*$C$11</f>
+        <f t="shared" si="0"/>
         <v>141387.7077</v>
       </c>
       <c r="D3" s="3">
         <v>160984</v>
       </c>
       <c r="E3" s="3">
-        <f t="shared" ref="E3:E7" si="0">C3-D3</f>
+        <f t="shared" ref="E3:E7" si="2">C3-D3</f>
         <v>-19596.292300000001</v>
       </c>
       <c r="F3">
-        <f>E3/$C$11</f>
+        <f t="shared" si="1"/>
         <v>-70.548627641573972</v>
       </c>
     </row>
@@ -582,18 +611,18 @@
         <v>67.09</v>
       </c>
       <c r="C4" s="3">
-        <f>B4*$C$11</f>
+        <f t="shared" si="0"/>
         <v>18635.5893</v>
       </c>
       <c r="D4" s="3">
         <v>15038</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3597.5892999999996</v>
       </c>
       <c r="F4">
-        <f>E4/$C$11</f>
+        <f t="shared" si="1"/>
         <v>12.951684127155559</v>
       </c>
     </row>
@@ -605,18 +634,18 @@
         <v>0.6</v>
       </c>
       <c r="C5" s="3">
-        <f>B5*$C$11</f>
+        <f t="shared" si="0"/>
         <v>166.66199999999998</v>
       </c>
       <c r="D5" s="3">
         <v>4506</v>
       </c>
       <c r="E5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>-4339.3379999999997</v>
       </c>
       <c r="F5">
-        <f>E5/$C$11</f>
+        <f t="shared" si="1"/>
         <v>-15.622054217518091</v>
       </c>
     </row>
@@ -628,18 +657,18 @@
         <v>16.690000000000001</v>
       </c>
       <c r="C6" s="3">
-        <f>B6*$C$11</f>
+        <f t="shared" si="0"/>
         <v>4635.9813000000004</v>
       </c>
       <c r="D6" s="3">
         <v>4233</v>
       </c>
       <c r="E6" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>402.98130000000037</v>
       </c>
       <c r="F6">
-        <f>E6/$C$11</f>
+        <f t="shared" si="1"/>
         <v>1.4507733016524478</v>
       </c>
     </row>
@@ -651,18 +680,18 @@
         <v>15.92</v>
       </c>
       <c r="C7" s="3">
-        <f>B7*$C$11</f>
-        <v>4422.0983999999999</v>
-      </c>
-      <c r="D7" s="3">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3">
         <f t="shared" si="0"/>
         <v>4422.0983999999999</v>
       </c>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="2"/>
+        <v>4422.0983999999999</v>
+      </c>
       <c r="F7">
-        <f>E7/$C$11</f>
+        <f t="shared" si="1"/>
         <v>15.92</v>
       </c>
     </row>
@@ -687,7 +716,7 @@
         <v>-20557.242399999988</v>
       </c>
       <c r="F8">
-        <f>E8/$C$11</f>
+        <f t="shared" si="1"/>
         <v>-74.008144868056263</v>
       </c>
     </row>
@@ -702,7 +731,134 @@
         <v>10</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <f>4.364+47.979</f>
+        <v>52.342999999999996</v>
+      </c>
+      <c r="C15">
+        <f>(3343+17179+32448)/1000</f>
+        <v>52.97</v>
+      </c>
+      <c r="D15">
+        <f>B15-C15</f>
+        <v>-0.62700000000000244</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>2.8319999999999999</v>
+      </c>
+      <c r="C16">
+        <v>2.8319999999999999</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ref="D16:D20" si="3">B16-C16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17">
+        <f>0.8+0.64</f>
+        <v>1.44</v>
+      </c>
+      <c r="C17">
+        <f>(80+1465+22)/1000</f>
+        <v>1.5669999999999999</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>-0.127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>1.5529999999999999</v>
+      </c>
+      <c r="C18">
+        <f>(542.3+580+250)/1000</f>
+        <v>1.3722999999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="3"/>
+        <v>0.18070000000000008</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>SUM(B15:B19)</f>
+        <v>58.167999999999992</v>
+      </c>
+      <c r="C20">
+        <f>SUM(C15:C19)</f>
+        <v>58.741300000000003</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="3"/>
+        <v>-0.57330000000001036</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B22" r:id="rId1" xr:uid="{88917467-013E-409E-AB73-BD684F29509C}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1097,7 +1253,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B6">
@@ -1265,7 +1421,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B6">

</xml_diff>